<commit_message>
Organizando las unidades desde las hojas de calculo
</commit_message>
<xml_diff>
--- a/codigo/repaso_matricial/general_2D/cercha_UribeEscamilla_11_3.xlsx
+++ b/codigo/repaso_matricial/general_2D/cercha_UribeEscamilla_11_3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,8 @@
     <sheet name="carga_distr" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="carga_punt" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="prop_mat" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="varios" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="config" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="varios" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="ang1" vbProcedure="false">varios!$B$1</definedName>
@@ -198,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t xml:space="preserve">nodo</t>
   </si>
@@ -258,6 +259,36 @@
   </si>
   <si>
     <t xml:space="preserve">rho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esc_def</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esc_faxial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esc_V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esc_M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U_FUER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U_LONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
   </si>
   <si>
     <t xml:space="preserve">ang1 = </t>
@@ -382,7 +413,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -415,6 +446,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,9 +473,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>289440</xdr:colOff>
+      <xdr:colOff>288000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -450,7 +485,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9977760" cy="9520200"/>
+          <a:ext cx="10029600" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -483,9 +518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>289440</xdr:colOff>
+      <xdr:colOff>288000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -495,7 +530,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9977760" cy="9520200"/>
+          <a:ext cx="10029600" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -533,9 +568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>689400</xdr:colOff>
+      <xdr:colOff>687960</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -545,7 +580,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9958680" cy="9520200"/>
+          <a:ext cx="10001520" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -578,9 +613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>689400</xdr:colOff>
+      <xdr:colOff>687960</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -590,7 +625,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9958680" cy="9520200"/>
+          <a:ext cx="10001520" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -628,9 +663,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>289440</xdr:colOff>
+      <xdr:colOff>288000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -640,7 +675,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9977760" cy="9520200"/>
+          <a:ext cx="10029600" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -673,9 +708,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>289440</xdr:colOff>
+      <xdr:colOff>288000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -685,7 +720,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9977760" cy="9520200"/>
+          <a:ext cx="10029600" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -718,9 +753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>289440</xdr:colOff>
+      <xdr:colOff>288000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -730,7 +765,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9977760" cy="9520200"/>
+          <a:ext cx="10029600" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -763,9 +798,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>289440</xdr:colOff>
+      <xdr:colOff>288000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -775,7 +810,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9977760" cy="9520200"/>
+          <a:ext cx="10029600" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -813,9 +848,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>289440</xdr:colOff>
+      <xdr:colOff>288000</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -825,7 +860,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9977760" cy="9520200"/>
+          <a:ext cx="10029600" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -858,9 +893,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>289440</xdr:colOff>
+      <xdr:colOff>288000</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -870,7 +905,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9977760" cy="9520200"/>
+          <a:ext cx="10029600" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -908,7 +943,7 @@
       <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1097,7 +1132,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.92"/>
   </cols>
@@ -1230,7 +1265,7 @@
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.01"/>
   </cols>
@@ -1353,7 +1388,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1482,7 +1517,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1550,11 +1585,11 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
@@ -1663,29 +1698,109 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B1" s="0" t="n">
         <f aca="false">ATAN2(4,3)</f>
         <v>0.643501108793284</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,21 +1810,21 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,13 +1832,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando soporte para apoyos inclinados
</commit_message>
<xml_diff>
--- a/codigo/repaso_matricial/general_2D/cercha_UribeEscamilla_11_3.xlsx
+++ b/codigo/repaso_matricial/general_2D/cercha_UribeEscamilla_11_3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -96,6 +96,19 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">m</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">grados</t>
         </r>
       </text>
     </comment>
@@ -199,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t xml:space="preserve">nodo</t>
   </si>
@@ -232,6 +245,9 @@
   </si>
   <si>
     <t xml:space="preserve">desplazamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotación</t>
   </si>
   <si>
     <t xml:space="preserve">b1</t>
@@ -322,11 +338,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.00E+00"/>
+    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -413,7 +430,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -434,7 +451,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -442,7 +463,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -473,9 +494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -485,7 +506,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10029600" cy="9518760"/>
+          <a:ext cx="10044720" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -518,9 +539,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -530,7 +551,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10029600" cy="9518760"/>
+          <a:ext cx="10044720" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -568,9 +589,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>687960</xdr:colOff>
+      <xdr:colOff>687600</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -580,7 +601,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10001520" cy="9518760"/>
+          <a:ext cx="10014120" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -613,9 +634,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>687960</xdr:colOff>
+      <xdr:colOff>687600</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -625,7 +646,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10001520" cy="9518760"/>
+          <a:ext cx="10014120" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -663,9 +684,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -675,7 +696,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10029600" cy="9518760"/>
+          <a:ext cx="10044720" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -708,9 +729,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -720,7 +741,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10029600" cy="9518760"/>
+          <a:ext cx="10044720" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -753,9 +774,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -765,7 +786,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10029600" cy="9518760"/>
+          <a:ext cx="10044720" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -798,9 +819,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -810,7 +831,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10029600" cy="9518760"/>
+          <a:ext cx="10044720" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -848,9 +869,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -860,7 +881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10029600" cy="9518760"/>
+          <a:ext cx="10044720" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -893,9 +914,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -905,7 +926,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10029600" cy="9518760"/>
+          <a:ext cx="10044720" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -943,7 +964,7 @@
       <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1132,7 +1153,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.92"/>
   </cols>
@@ -1259,18 +1280,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.01"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,6 +1300,9 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,6 +1316,9 @@
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1304,6 +1331,9 @@
       <c r="C3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1316,6 +1346,9 @@
       <c r="C4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -1327,6 +1360,10 @@
       <c r="C5" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="D5" s="5" t="e">
+        <f aca="false">NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -1338,8 +1375,12 @@
       <c r="C6" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="5" t="e">
+        <f aca="false">NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>3</v>
       </c>
@@ -1349,8 +1390,12 @@
       <c r="C7" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="5" t="e">
+        <f aca="false">NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>4</v>
       </c>
@@ -1360,7 +1405,12 @@
       <c r="C8" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
+      <c r="D8" s="5" t="e">
+        <f aca="false">NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1388,23 +1438,23 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1412,16 +1462,16 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="n">
+      <c r="B2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1429,16 +1479,16 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="n">
+      <c r="B3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1446,16 +1496,16 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5" t="n">
+      <c r="B4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1463,16 +1513,16 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="n">
+      <c r="B5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1480,16 +1530,16 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="n">
+      <c r="B6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1517,7 +1567,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1527,7 +1577,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1589,41 +1639,41 @@
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="E1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="8" t="n">
         <v>2040</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="8" t="n">
         <f aca="false">C2^2/12</f>
         <v>75</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1631,17 +1681,17 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="8" t="n">
         <v>2040</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="8" t="n">
         <f aca="false">C3^2/12</f>
         <v>133.333333333333</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1649,17 +1699,17 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="8" t="n">
         <v>2040</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="8" t="n">
         <f aca="false">C4^2/12</f>
         <v>833.333333333333</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1667,17 +1717,17 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="8" t="n">
         <v>2040</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="8" t="n">
         <f aca="false">C5^2/12</f>
         <v>1875</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1700,47 +1750,47 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>23</v>
+      <c r="A3" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>24</v>
+      <c r="A4" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>25</v>
+      <c r="A5" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.05</v>
@@ -1748,18 +1798,18 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1784,23 +1834,23 @@
       <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1" s="0" t="n">
         <f aca="false">ATAN2(4,3)</f>
         <v>0.643501108793284</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,21 +1860,21 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1832,13 +1882,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>